<commit_message>
Feature/dathpq2/update unit test (#101)
* update unit test

* update import file excel

* update unit test

* update import topic

* update import

* https

---------

Co-authored-by: sechmachine <groovykermit@outlook.com>
</commit_message>
<xml_diff>
--- a/Template_Import_Syllabus.xlsx
+++ b/Template_Import_Syllabus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSA\Project\fms-backend-api\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSA\Project\fms-backend-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D4C47-8560-40F2-825C-45A68624BE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CB1773-A11E-4F0D-B637-D3085AB70021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,7 +979,7 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>TEEST</t>
+    <t>TEEST123123123</t>
   </si>
 </sst>
 </file>
@@ -1772,6 +1772,9 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1838,24 +1841,30 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="13" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1865,12 +1874,6 @@
     <xf numFmtId="165" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1906,9 +1909,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2627,22 +2627,22 @@
       <c r="O10" s="23"/>
     </row>
     <row r="11" spans="2:15" s="26" customFormat="1" ht="17.399999999999999">
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="96"/>
-      <c r="N11" s="96"/>
-      <c r="O11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="97"/>
+      <c r="O11" s="98"/>
     </row>
     <row r="12" spans="2:15" s="26" customFormat="1" ht="18">
       <c r="B12" s="27"/>
@@ -2661,22 +2661,22 @@
       <c r="O12" s="30"/>
     </row>
     <row r="13" spans="2:15" s="26" customFormat="1" ht="24.6">
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="99" t="s">
         <v>174</v>
       </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
-      <c r="O13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="101"/>
     </row>
     <row r="14" spans="2:15" ht="14.4">
       <c r="B14" s="25"/>
@@ -2731,16 +2731,16 @@
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="101" t="s">
+      <c r="F17" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="103" t="s">
+      <c r="G17" s="103"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="103"/>
-      <c r="K17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="105"/>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
@@ -2751,16 +2751,16 @@
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
-      <c r="F18" s="105" t="s">
+      <c r="F18" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="107" t="s">
+      <c r="G18" s="107"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="J18" s="107"/>
-      <c r="K18" s="108"/>
+      <c r="J18" s="108"/>
+      <c r="K18" s="109"/>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
@@ -2771,16 +2771,16 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="92" t="s">
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="93"/>
-      <c r="K19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="95"/>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
@@ -2941,7 +2941,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -2959,15 +2959,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1">
-      <c r="A1" s="109" t="str">
+      <c r="A1" s="110" t="str">
         <f>C3&amp;" "&amp;"Syllabus"</f>
         <v>TEST Syllabus</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" customHeight="1">
       <c r="A2" s="81">
@@ -2977,7 +2977,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="115" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D2" s="116"/>
       <c r="E2" s="116"/>
@@ -2990,12 +2990,12 @@
       <c r="B3" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="118" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="113"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="120"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1">
       <c r="A4" s="83">
@@ -3004,12 +3004,12 @@
       <c r="B4" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="114" t="s">
+      <c r="C4" s="118" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="113"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="120"/>
     </row>
     <row r="5" spans="1:6" ht="18.600000000000001" customHeight="1">
       <c r="A5" s="83">
@@ -3018,18 +3018,18 @@
       <c r="B5" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="118">
+      <c r="C5" s="121">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="120"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="32.4" customHeight="1">
-      <c r="A6" s="110">
+      <c r="A6" s="111">
         <v>5</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="112" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="85" t="s">
@@ -3046,8 +3046,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="26.4">
-      <c r="A7" s="110"/>
-      <c r="B7" s="111"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="85" t="s">
         <v>10</v>
       </c>
@@ -3062,8 +3062,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="27.6" customHeight="1">
-      <c r="A8" s="110"/>
-      <c r="B8" s="111"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="85" t="s">
         <v>31</v>
       </c>
@@ -3073,13 +3073,13 @@
       <c r="E8" s="88">
         <v>28</v>
       </c>
-      <c r="F8" s="135" t="s">
+      <c r="F8" s="90" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.6" customHeight="1">
-      <c r="A9" s="110"/>
-      <c r="B9" s="111"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="85" t="s">
         <v>32</v>
       </c>
@@ -3089,23 +3089,23 @@
       <c r="E9" s="88">
         <v>42</v>
       </c>
-      <c r="F9" s="135" t="s">
+      <c r="F9" s="90" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="46.2" customHeight="1">
-      <c r="A10" s="110"/>
-      <c r="B10" s="111"/>
+      <c r="A10" s="111"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="89" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="86">
         <v>6</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="113" t="s">
         <v>172</v>
       </c>
-      <c r="F10" s="122"/>
+      <c r="F10" s="114"/>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="34" t="s">
@@ -3359,14 +3359,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B6:B10"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
@@ -3412,24 +3412,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A1" s="132" t="str">
+      <c r="A1" s="133" t="str">
         <f>Syllabus!C3 &amp; " - Training Schedule"</f>
         <v>TEST - Training Schedule</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
     </row>
     <row r="2" spans="1:9" ht="39" customHeight="1">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="134"/>
+      <c r="B2" s="135"/>
       <c r="C2" s="36" t="s">
         <v>82</v>
       </c>
@@ -3453,13 +3453,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="125">
+      <c r="A3" s="126">
         <v>1</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="129">
+      <c r="C3" s="130">
         <v>1</v>
       </c>
       <c r="D3" s="40" t="s">
@@ -3482,9 +3482,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="79.2">
-      <c r="A4" s="126"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="127"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="131"/>
       <c r="D4" s="5" t="s">
         <v>87</v>
       </c>
@@ -3505,9 +3505,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="79.2">
-      <c r="A5" s="126"/>
-      <c r="B5" s="128"/>
-      <c r="C5" s="131">
+      <c r="A5" s="127"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="132">
         <v>2</v>
       </c>
       <c r="D5" s="45" t="s">
@@ -3530,9 +3530,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="26.4">
-      <c r="A6" s="126"/>
-      <c r="B6" s="128"/>
-      <c r="C6" s="131"/>
+      <c r="A6" s="127"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="132"/>
       <c r="D6" s="45" t="s">
         <v>89</v>
       </c>
@@ -3553,9 +3553,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="158.4">
-      <c r="A7" s="126"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="131"/>
+      <c r="A7" s="127"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="132"/>
       <c r="D7" s="46" t="s">
         <v>90</v>
       </c>
@@ -3576,9 +3576,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="79.2">
-      <c r="A8" s="126"/>
-      <c r="B8" s="128"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="127"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
@@ -3599,9 +3599,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="26.4">
-      <c r="A9" s="126"/>
-      <c r="B9" s="128"/>
-      <c r="C9" s="130"/>
+      <c r="A9" s="127"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="131"/>
       <c r="D9" s="51" t="s">
         <v>89</v>
       </c>
@@ -3622,13 +3622,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="125">
+      <c r="A10" s="126">
         <v>2</v>
       </c>
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="129">
+      <c r="C10" s="130">
         <v>3</v>
       </c>
       <c r="D10" s="53" t="s">
@@ -3651,9 +3651,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="132">
-      <c r="A11" s="126"/>
-      <c r="B11" s="128"/>
-      <c r="C11" s="130"/>
+      <c r="A11" s="127"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="131"/>
       <c r="D11" s="5" t="s">
         <v>94</v>
       </c>
@@ -3674,9 +3674,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="79.2">
-      <c r="A12" s="126"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="131">
+      <c r="A12" s="127"/>
+      <c r="B12" s="129"/>
+      <c r="C12" s="132">
         <v>4</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -3699,9 +3699,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="26.4">
-      <c r="A13" s="126"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="127"/>
+      <c r="B13" s="129"/>
+      <c r="C13" s="131"/>
       <c r="D13" s="45" t="s">
         <v>89</v>
       </c>
@@ -3722,13 +3722,13 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="125">
+      <c r="A14" s="126">
         <v>3</v>
       </c>
-      <c r="B14" s="123" t="s">
+      <c r="B14" s="124" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="129">
+      <c r="C14" s="130">
         <v>5</v>
       </c>
       <c r="D14" s="54" t="s">
@@ -3751,9 +3751,9 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="126"/>
-      <c r="B15" s="128"/>
-      <c r="C15" s="131"/>
+      <c r="A15" s="127"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="132"/>
       <c r="D15" s="53" t="s">
         <v>93</v>
       </c>
@@ -3772,9 +3772,9 @@
       <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:9" ht="39.6">
-      <c r="A16" s="126"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="127"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="131"/>
       <c r="D16" s="53" t="s">
         <v>98</v>
       </c>
@@ -3795,9 +3795,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="79.2">
-      <c r="A17" s="126"/>
-      <c r="B17" s="128"/>
-      <c r="C17" s="129">
+      <c r="A17" s="127"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130">
         <v>6</v>
       </c>
       <c r="D17" s="45" t="s">
@@ -3820,9 +3820,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="52.8">
-      <c r="A18" s="126"/>
-      <c r="B18" s="128"/>
-      <c r="C18" s="131"/>
+      <c r="A18" s="127"/>
+      <c r="B18" s="129"/>
+      <c r="C18" s="132"/>
       <c r="D18" s="45" t="s">
         <v>100</v>
       </c>
@@ -3843,9 +3843,9 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="26.4">
-      <c r="A19" s="126"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="130"/>
+      <c r="A19" s="127"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="131"/>
       <c r="D19" s="45" t="s">
         <v>89</v>
       </c>
@@ -3866,13 +3866,13 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="125">
+      <c r="A20" s="126">
         <v>4</v>
       </c>
-      <c r="B20" s="123" t="s">
+      <c r="B20" s="124" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="129">
+      <c r="C20" s="130">
         <v>7</v>
       </c>
       <c r="D20" s="53" t="s">
@@ -3895,9 +3895,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="39.6">
-      <c r="A21" s="126"/>
-      <c r="B21" s="128"/>
-      <c r="C21" s="130"/>
+      <c r="A21" s="127"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="131"/>
       <c r="D21" s="53" t="s">
         <v>102</v>
       </c>
@@ -3918,9 +3918,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="79.2">
-      <c r="A22" s="126"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="131">
+      <c r="A22" s="127"/>
+      <c r="B22" s="129"/>
+      <c r="C22" s="132">
         <v>8</v>
       </c>
       <c r="D22" s="45" t="s">
@@ -3943,9 +3943,9 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="52.8">
-      <c r="A23" s="126"/>
-      <c r="B23" s="128"/>
-      <c r="C23" s="131"/>
+      <c r="A23" s="127"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="132"/>
       <c r="D23" s="45" t="s">
         <v>104</v>
       </c>
@@ -3966,9 +3966,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="26.4">
-      <c r="A24" s="126"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="130"/>
+      <c r="A24" s="127"/>
+      <c r="B24" s="129"/>
+      <c r="C24" s="131"/>
       <c r="D24" s="45" t="s">
         <v>89</v>
       </c>
@@ -3989,13 +3989,13 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="125">
+      <c r="A25" s="126">
         <v>5</v>
       </c>
-      <c r="B25" s="123" t="s">
+      <c r="B25" s="124" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="129">
+      <c r="C25" s="130">
         <v>9</v>
       </c>
       <c r="D25" s="53" t="s">
@@ -4018,9 +4018,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="79.2">
-      <c r="A26" s="126"/>
-      <c r="B26" s="128"/>
-      <c r="C26" s="130"/>
+      <c r="A26" s="127"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="131"/>
       <c r="D26" s="55" t="s">
         <v>106</v>
       </c>
@@ -4041,9 +4041,9 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="26.4">
-      <c r="A27" s="126"/>
-      <c r="B27" s="128"/>
-      <c r="C27" s="131">
+      <c r="A27" s="127"/>
+      <c r="B27" s="129"/>
+      <c r="C27" s="132">
         <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -4066,9 +4066,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="79.2">
-      <c r="A28" s="126"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="131"/>
+      <c r="A28" s="127"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="45" t="s">
         <v>109</v>
       </c>
@@ -4089,9 +4089,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="26.4">
-      <c r="A29" s="126"/>
-      <c r="B29" s="128"/>
-      <c r="C29" s="130"/>
+      <c r="A29" s="127"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="131"/>
       <c r="D29" s="45" t="s">
         <v>89</v>
       </c>
@@ -4112,13 +4112,13 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="125">
+      <c r="A30" s="126">
         <v>6</v>
       </c>
-      <c r="B30" s="123" t="s">
+      <c r="B30" s="124" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="129">
+      <c r="C30" s="130">
         <v>11</v>
       </c>
       <c r="D30" s="53" t="s">
@@ -4141,9 +4141,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="52.8">
-      <c r="A31" s="126"/>
-      <c r="B31" s="126"/>
-      <c r="C31" s="130"/>
+      <c r="A31" s="127"/>
+      <c r="B31" s="127"/>
+      <c r="C31" s="131"/>
       <c r="D31" s="56" t="s">
         <v>158</v>
       </c>
@@ -4164,9 +4164,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="39.6">
-      <c r="A32" s="126"/>
-      <c r="B32" s="126"/>
-      <c r="C32" s="129">
+      <c r="A32" s="127"/>
+      <c r="B32" s="127"/>
+      <c r="C32" s="130">
         <v>12</v>
       </c>
       <c r="D32" s="79" t="s">
@@ -4189,9 +4189,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="79.2">
-      <c r="A33" s="126"/>
-      <c r="B33" s="126"/>
-      <c r="C33" s="131"/>
+      <c r="A33" s="127"/>
+      <c r="B33" s="127"/>
+      <c r="C33" s="132"/>
       <c r="D33" s="57" t="s">
         <v>111</v>
       </c>
@@ -4212,9 +4212,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="52.8">
-      <c r="A34" s="126"/>
-      <c r="B34" s="126"/>
-      <c r="C34" s="131"/>
+      <c r="A34" s="127"/>
+      <c r="B34" s="127"/>
+      <c r="C34" s="132"/>
       <c r="D34" s="45" t="s">
         <v>112</v>
       </c>
@@ -4235,9 +4235,9 @@
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="126"/>
-      <c r="B35" s="126"/>
-      <c r="C35" s="130"/>
+      <c r="A35" s="127"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="131"/>
       <c r="D35" s="45" t="s">
         <v>89</v>
       </c>
@@ -4256,13 +4256,13 @@
       <c r="I35" s="75"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="125">
+      <c r="A36" s="126">
         <v>7</v>
       </c>
-      <c r="B36" s="123" t="s">
+      <c r="B36" s="124" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="123">
+      <c r="C36" s="124">
         <v>13</v>
       </c>
       <c r="D36" s="40" t="s">
@@ -4285,9 +4285,9 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="126"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="128"/>
+      <c r="A37" s="127"/>
+      <c r="B37" s="129"/>
+      <c r="C37" s="129"/>
       <c r="D37" s="54" t="s">
         <v>114</v>
       </c>
@@ -4308,9 +4308,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="39.6">
-      <c r="A38" s="126"/>
-      <c r="B38" s="128"/>
-      <c r="C38" s="124"/>
+      <c r="A38" s="127"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="125"/>
       <c r="D38" s="56" t="s">
         <v>163</v>
       </c>
@@ -4331,9 +4331,9 @@
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="126"/>
-      <c r="B39" s="128"/>
-      <c r="C39" s="128">
+      <c r="A39" s="127"/>
+      <c r="B39" s="129"/>
+      <c r="C39" s="129">
         <v>14</v>
       </c>
       <c r="D39" s="56" t="s">
@@ -4356,9 +4356,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="52.8">
-      <c r="A40" s="126"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="128"/>
+      <c r="A40" s="127"/>
+      <c r="B40" s="129"/>
+      <c r="C40" s="129"/>
       <c r="D40" s="45" t="s">
         <v>115</v>
       </c>
@@ -4379,9 +4379,9 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="26.4">
-      <c r="A41" s="126"/>
-      <c r="B41" s="128"/>
-      <c r="C41" s="124"/>
+      <c r="A41" s="127"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="125"/>
       <c r="D41" s="45" t="s">
         <v>89</v>
       </c>
@@ -4402,13 +4402,13 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="125">
+      <c r="A42" s="126">
         <v>8</v>
       </c>
-      <c r="B42" s="123" t="s">
+      <c r="B42" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="123">
+      <c r="C42" s="124">
         <v>15</v>
       </c>
       <c r="D42" s="40" t="s">
@@ -4431,9 +4431,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="52.8">
-      <c r="A43" s="126"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="124"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="125"/>
       <c r="D43" s="56" t="s">
         <v>164</v>
       </c>
@@ -4454,9 +4454,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="39.6">
-      <c r="A44" s="126"/>
-      <c r="B44" s="128"/>
-      <c r="C44" s="128">
+      <c r="A44" s="127"/>
+      <c r="B44" s="129"/>
+      <c r="C44" s="129">
         <v>16</v>
       </c>
       <c r="D44" s="56" t="s">
@@ -4479,9 +4479,9 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="52.8">
-      <c r="A45" s="126"/>
-      <c r="B45" s="128"/>
-      <c r="C45" s="128"/>
+      <c r="A45" s="127"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="129"/>
       <c r="D45" s="45" t="s">
         <v>117</v>
       </c>
@@ -4502,9 +4502,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="26.4">
-      <c r="A46" s="126"/>
-      <c r="B46" s="128"/>
-      <c r="C46" s="124"/>
+      <c r="A46" s="127"/>
+      <c r="B46" s="129"/>
+      <c r="C46" s="125"/>
       <c r="D46" s="45" t="s">
         <v>89</v>
       </c>
@@ -4525,13 +4525,13 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="125">
+      <c r="A47" s="126">
         <v>9</v>
       </c>
-      <c r="B47" s="123" t="s">
+      <c r="B47" s="124" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="123">
+      <c r="C47" s="124">
         <v>17</v>
       </c>
       <c r="D47" s="40" t="s">
@@ -4554,9 +4554,9 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="126"/>
-      <c r="B48" s="128"/>
-      <c r="C48" s="128"/>
+      <c r="A48" s="127"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="129"/>
       <c r="D48" s="54" t="s">
         <v>119</v>
       </c>
@@ -4577,9 +4577,9 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="57" customHeight="1">
-      <c r="A49" s="126"/>
-      <c r="B49" s="128"/>
-      <c r="C49" s="124"/>
+      <c r="A49" s="127"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="125"/>
       <c r="D49" s="56" t="s">
         <v>166</v>
       </c>
@@ -4600,9 +4600,9 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="39.6">
-      <c r="A50" s="126"/>
-      <c r="B50" s="128"/>
-      <c r="C50" s="123">
+      <c r="A50" s="127"/>
+      <c r="B50" s="129"/>
+      <c r="C50" s="124">
         <v>18</v>
       </c>
       <c r="D50" s="56" t="s">
@@ -4625,9 +4625,9 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="52.8">
-      <c r="A51" s="126"/>
-      <c r="B51" s="128"/>
-      <c r="C51" s="128"/>
+      <c r="A51" s="127"/>
+      <c r="B51" s="129"/>
+      <c r="C51" s="129"/>
       <c r="D51" s="45" t="s">
         <v>120</v>
       </c>
@@ -4648,9 +4648,9 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="26.4">
-      <c r="A52" s="126"/>
-      <c r="B52" s="128"/>
-      <c r="C52" s="124"/>
+      <c r="A52" s="127"/>
+      <c r="B52" s="129"/>
+      <c r="C52" s="125"/>
       <c r="D52" s="45" t="s">
         <v>89</v>
       </c>
@@ -4671,13 +4671,13 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="52.8" customHeight="1">
-      <c r="A53" s="125">
+      <c r="A53" s="126">
         <v>10</v>
       </c>
-      <c r="B53" s="123" t="s">
+      <c r="B53" s="124" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="123">
+      <c r="C53" s="124">
         <v>19</v>
       </c>
       <c r="D53" s="40" t="s">
@@ -4700,9 +4700,9 @@
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="126"/>
-      <c r="B54" s="128"/>
-      <c r="C54" s="128"/>
+      <c r="A54" s="127"/>
+      <c r="B54" s="129"/>
+      <c r="C54" s="129"/>
       <c r="D54" s="55" t="s">
         <v>121</v>
       </c>
@@ -4723,9 +4723,9 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="79.2">
-      <c r="A55" s="126"/>
-      <c r="B55" s="128"/>
-      <c r="C55" s="124"/>
+      <c r="A55" s="127"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="125"/>
       <c r="D55" s="45" t="s">
         <v>122</v>
       </c>
@@ -4746,9 +4746,9 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="13.8">
-      <c r="A56" s="126"/>
-      <c r="B56" s="128"/>
-      <c r="C56" s="123">
+      <c r="A56" s="127"/>
+      <c r="B56" s="129"/>
+      <c r="C56" s="124">
         <v>20</v>
       </c>
       <c r="D56" s="45" t="s">
@@ -4771,9 +4771,9 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="52.8">
-      <c r="A57" s="126"/>
-      <c r="B57" s="128"/>
-      <c r="C57" s="128"/>
+      <c r="A57" s="127"/>
+      <c r="B57" s="129"/>
+      <c r="C57" s="129"/>
       <c r="D57" s="45" t="s">
         <v>123</v>
       </c>
@@ -4794,9 +4794,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="26.4">
-      <c r="A58" s="126"/>
-      <c r="B58" s="128"/>
-      <c r="C58" s="124"/>
+      <c r="A58" s="127"/>
+      <c r="B58" s="129"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="45" t="s">
         <v>89</v>
       </c>
@@ -4817,13 +4817,13 @@
       </c>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="125">
+      <c r="A59" s="126">
         <v>11</v>
       </c>
-      <c r="B59" s="123" t="s">
+      <c r="B59" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="123">
+      <c r="C59" s="124">
         <v>21</v>
       </c>
       <c r="D59" s="60" t="s">
@@ -4846,9 +4846,9 @@
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="126"/>
-      <c r="B60" s="128"/>
-      <c r="C60" s="128"/>
+      <c r="A60" s="127"/>
+      <c r="B60" s="129"/>
+      <c r="C60" s="129"/>
       <c r="D60" s="54" t="s">
         <v>125</v>
       </c>
@@ -4870,9 +4870,9 @@
       <c r="K60" s="16"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="126"/>
-      <c r="B61" s="128"/>
-      <c r="C61" s="128"/>
+      <c r="A61" s="127"/>
+      <c r="B61" s="129"/>
+      <c r="C61" s="129"/>
       <c r="D61" s="55" t="s">
         <v>124</v>
       </c>
@@ -4893,9 +4893,9 @@
       </c>
     </row>
     <row r="62" spans="1:11" ht="26.4">
-      <c r="A62" s="126"/>
-      <c r="B62" s="128"/>
-      <c r="C62" s="128"/>
+      <c r="A62" s="127"/>
+      <c r="B62" s="129"/>
+      <c r="C62" s="129"/>
       <c r="D62" s="45" t="s">
         <v>126</v>
       </c>
@@ -4916,9 +4916,9 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="26.4">
-      <c r="A63" s="126"/>
-      <c r="B63" s="128"/>
-      <c r="C63" s="124"/>
+      <c r="A63" s="127"/>
+      <c r="B63" s="129"/>
+      <c r="C63" s="125"/>
       <c r="D63" s="45" t="s">
         <v>127</v>
       </c>
@@ -4939,9 +4939,9 @@
       </c>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="126"/>
-      <c r="B64" s="128"/>
-      <c r="C64" s="123">
+      <c r="A64" s="127"/>
+      <c r="B64" s="129"/>
+      <c r="C64" s="124">
         <v>22</v>
       </c>
       <c r="D64" s="61" t="s">
@@ -4964,9 +4964,9 @@
       </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="127"/>
-      <c r="B65" s="124"/>
-      <c r="C65" s="124"/>
+      <c r="A65" s="128"/>
+      <c r="B65" s="125"/>
+      <c r="C65" s="125"/>
       <c r="D65" s="61" t="s">
         <v>18</v>
       </c>
@@ -4987,7 +4987,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" customHeight="1">
-      <c r="A66" s="125">
+      <c r="A66" s="126">
         <v>12</v>
       </c>
       <c r="B66" s="59" t="s">
@@ -5016,11 +5016,11 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="15" customHeight="1">
-      <c r="A67" s="126"/>
+      <c r="A67" s="127"/>
       <c r="B67" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="128">
+      <c r="C67" s="129">
         <v>24</v>
       </c>
       <c r="D67" s="55" t="s">
@@ -5043,9 +5043,9 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="15" customHeight="1">
-      <c r="A68" s="127"/>
+      <c r="A68" s="128"/>
       <c r="B68" s="80"/>
-      <c r="C68" s="124"/>
+      <c r="C68" s="125"/>
       <c r="D68" s="55" t="s">
         <v>133</v>
       </c>

</xml_diff>